<commit_message>
220612 SW: serializer update and mypage udpate
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t>2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -746,7 +746,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -902,6 +902,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1222,34 +1225,34 @@
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
@@ -1935,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2149,7 +2152,9 @@
       <c r="D20" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="F20" s="43"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -2160,7 +2165,9 @@
       <c r="D21" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="43"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
220612 SW: mypage test
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -383,6 +383,10 @@
   </si>
   <si>
     <t>팀 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2061,7 +2065,9 @@
       <c r="D11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="F11" s="17"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -2072,7 +2078,9 @@
       <c r="D12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
220613 SW: TeamPage Update
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -1942,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
220614 SW: mypage test completed
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -750,7 +750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -906,6 +906,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1229,34 +1232,34 @@
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="57"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="55"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
@@ -1943,7 +1946,7 @@
   <dimension ref="B1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2118,7 +2121,9 @@
       <c r="D16" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="42"/>
+      <c r="E16" s="53" t="s">
+        <v>65</v>
+      </c>
       <c r="F16" s="43"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -2129,7 +2134,9 @@
       <c r="D17" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="42"/>
+      <c r="E17" s="53" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="43"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -2140,7 +2147,9 @@
       <c r="D18" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="53" t="s">
+        <v>65</v>
+      </c>
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
220624 SW: pjt plannig modified
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\ssafy\pjt\Find_Dev_Team\기획\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIWON\Desktop\SSAFY\04_프로젝트\02_Find_Dev_Team\기획\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
     <sheet name="기능명세서" sheetId="2" r:id="rId2"/>
+    <sheet name="구현서비스" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="136">
   <si>
     <t>2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -171,10 +172,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>랜딩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인/회원가입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -263,26 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>account/login/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account/signup/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account/logout/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account/password/rest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>accounts/signout/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>메인 페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -299,10 +276,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>teams/&lt;int: team_pk&gt;/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자 북마크</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -311,18 +284,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adapter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>accounts/&lt;int:user_pk&gt;/mypage/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 사용자 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>개별 사용자 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -339,11 +300,204 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체 팀 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teams/</t>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>2.1.5</t>
+  </si>
+  <si>
+    <t>2.1.6</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>로그인 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 프로필 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/user/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 팀/사용자 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/login/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/signup/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/logout/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/password/rest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/accounts/&lt;int:user_pk&gt;/mypage/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/accounts/&lt;int:user_pk&gt;/mypage/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/accounts/signout/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/teams/&lt;int: team_pk&gt;/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/teams/create/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현서비스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 페이지 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 생성(팀이 없을 경우)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이 페이지 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>권한(로그인/팀장 등)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 페이지(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 페이지 이동(로그인 성공 시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원인별 로그인 에러 출력(로그인 실패 시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 페이지 이동(회원 가입 성공 시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원인별 회원 가입 에러 출력(회원 가입 실패 시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 프로필 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로필 수정 페이지(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크 모아보기(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프론트/백엔드 카운팅 필요</t>
+  </si>
+  <si>
+    <t>체크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로필 수정 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로필 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 페이지</t>
+  </si>
+  <si>
+    <t>비밀번호 변경 페이지(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 변경 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 변경</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -351,42 +505,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>teams/&lt;int: team_pk&gt;/teampage/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.3</t>
-  </si>
-  <si>
-    <t>2.1.4</t>
-  </si>
-  <si>
-    <t>2.1.5</t>
-  </si>
-  <si>
-    <t>2.1.6</t>
-  </si>
-  <si>
-    <t>2.2.4</t>
-  </si>
-  <si>
-    <t>로그인 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>팀 페이지</t>
+    <t>마이 팀 페이지 이동(팀이 있을 경우)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 수정 페이지(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 생성 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이 팀 페이지 이동(팀 생성 성공 시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인이 필요한 서비스입니다 메시지 알림 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개별 팀 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개별 멤버 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크</t>
+  </si>
+  <si>
+    <t>개별 팀 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개별 멤버 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체/개별 멤버 페이지(모달)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체/개별 팀 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,25 +613,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="12"/>
-      <color theme="1"/>
       <name val="맑은 고딕"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,8 +702,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8D1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -675,11 +883,50 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -687,16 +934,130 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -712,36 +1073,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -750,7 +1096,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -799,29 +1145,101 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -829,100 +1247,190 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,9 +1441,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE8D1FF"/>
+      <color rgb="FFFFE7FF"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFE2C5FF"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFCC99FF"/>
-      <color rgb="FFCCCCFF"/>
       <color rgb="FF9966FF"/>
     </mruColors>
   </colors>
@@ -1232,34 +1745,34 @@
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="57"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
@@ -1318,42 +1831,42 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="31"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="31"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
@@ -1363,16 +1876,16 @@
         <v>12</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="31"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
@@ -1382,137 +1895,137 @@
         <v>14</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="31"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="31"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="31"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="31"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="31"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="31"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="31"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="31"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
@@ -1521,17 +2034,17 @@
       <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="31"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
@@ -1540,112 +2053,112 @@
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="31"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="18"/>
+        <v>48</v>
+      </c>
+      <c r="D19" s="16"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="31"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="D20" s="16"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="31"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="23"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="D21" s="16"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="31"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="23"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="D22" s="16"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="31"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="23"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="D23" s="16"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="31"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="23"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
@@ -1654,127 +2167,127 @@
       <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="31"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="23"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+        <v>73</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="31"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="23"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="31"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="23"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+        <v>75</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="10"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="31"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="23"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="31"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="23"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="31"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="23"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="31"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="23"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
@@ -1783,70 +2296,70 @@
       <c r="C31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="31"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="23"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="31"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="23"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="31"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="23"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="31"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="23"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="12" t="s">
@@ -1855,51 +2368,51 @@
       <c r="C35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="31"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="23"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="31"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="23"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="48"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="40"/>
     </row>
     <row r="38" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
@@ -1908,17 +2421,17 @@
       <c r="C38" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="49"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="41"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
@@ -1943,10 +2456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F23"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1968,246 +2481,622 @@
     </row>
     <row r="3" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
+      <c r="E5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>71</v>
-      </c>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="17"/>
+        <v>85</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="17"/>
+        <v>86</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="17"/>
+        <v>87</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="32"/>
+      <c r="C16" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="35"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="32"/>
+      <c r="C17" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="32"/>
+      <c r="C18" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="43"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="40"/>
-      <c r="C17" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="43"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="43"/>
+      <c r="E18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="43"/>
+      <c r="D20" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="43"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="51" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-    </row>
-    <row r="23" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="23"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
+      <c r="D21" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="35"/>
+    </row>
+    <row r="22" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="19"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="44.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="59.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="111" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="88" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="52"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="59"/>
+      <c r="E10" s="89"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="59"/>
+      <c r="E11" s="89"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="89"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="60"/>
+      <c r="E13" s="97" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="72"/>
+      <c r="C14" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="60"/>
+      <c r="E14" s="97" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="72"/>
+      <c r="C15" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="90"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="70"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="90"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="74"/>
+      <c r="C18" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="61"/>
+      <c r="E18" s="91"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="75"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="91"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="99" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="77"/>
+      <c r="C21" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="92"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="77"/>
+      <c r="C22" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="92"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="78"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="92"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="93"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="80"/>
+      <c r="C25" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="93"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="81"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="93"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="94"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="83"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="94"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="84" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="95"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="85"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="95"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="86" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="86"/>
+      <c r="C32" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="86"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="96"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="108" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="108"/>
+      <c r="E34" s="109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="110"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="109"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="102"/>
+      <c r="E36" s="103"/>
+    </row>
+    <row r="37" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="104"/>
+      <c r="C37" s="105" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="105"/>
+      <c r="E37" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B28"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
220701 hj: css update
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -17,7 +17,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="173">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
+  <x:si>
+    <x:t>비밀번호 변경 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 생성 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 팀 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>나의 프로필 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 페이지 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가 기능 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 페이지 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 팀/사용자 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>원인별 에러 출력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>페이지 전환 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로세스/태스크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>배포 및 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인/회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크 모아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지 이동(팀이 있을 경우)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지 이동(팀 생성 성공 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/teams/&lt;int: team_pk&gt;/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인 페이지 이동(회원 가입 성공 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 로그아웃 완료 alert창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>원인별 로그인 에러 출력(로그인 실패 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/password/rest</x:t>
+  </x:si>
   <x:si>
     <x:t>개인카드 상세조회</x:t>
   </x:si>
@@ -28,514 +91,454 @@
     <x:t>팀 페이지 수정</x:t>
   </x:si>
   <x:si>
+    <x:t>북마크 등록 해제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 멤버 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 수정/조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀장 등록 해제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 사용자 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/&lt;int: user_pk&gt;/bookmark/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀원이 모두 모집되었을 경우, 해당 팀 카드는 메인에서 제외</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/&lt;int:user_pk&gt;/mypage/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 사용자 조회/개별 사용자 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 완료 alert 창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/logout/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/signup/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/signout/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 마이 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 메인 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀을 만드는 유저가 팀장이 됨</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인페이지에 해당 팀 추가 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체/개별 멤버 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인 페이지 이동(로그인 성공 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인/로그아웃/회원가입/회원탈퇴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 마이 팀 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RESTful url/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.</x:t>
+  </x:si>
+  <x:si>
     <x:t>X</x:t>
   </x:si>
   <x:si>
+    <x:t>디자인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>배포</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nav</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>백엔드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>api</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모델링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀장</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>조건</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>체크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 생성(팀이 없을 경우)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/user/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 수정 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쪽지 보내기/채팅/오픈챗팅</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프론트/백엔드 카운팅 필요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/login/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>권한(로그인/팀장 등)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크 모아보기(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>드롭다운으로 데이터 출력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 페이지 생성/수정/조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인페이지에 유저 추가 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 프로필 수정 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navbar 페이지연결</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통합 기능 테스트 및 디버깅</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/teams/create/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 변경 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
     <x:t>부가기능 3</x:t>
   </x:si>
   <x:si>
+    <x:t>check</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능명세서</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.3.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프론트엔드</x:t>
+  </x:si>
+  <x:si>
     <x:t>메인기능</x:t>
   </x:si>
   <x:si>
-    <x:t>메인페이지에 해당 팀 추가 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쪽지 보내기/채팅/오픈챗팅</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>권한(로그인/팀장 등)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성(팀이 없을 경우)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/login/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/user/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 모아보기(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 수정 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프론트/백엔드 카운팅 필요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/teams/create/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통합 기능 테스트 및 디버깅</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 변경 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 페이지 생성/수정/조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 프로필 수정 페이지</x:t>
+    <x:t>로그인페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인여부</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 찾기</x:t>
   </x:si>
   <x:si>
     <x:t>북마크 기능</x:t>
   </x:si>
   <x:si>
-    <x:t>로그인페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 완료 alert 창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nav</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 마이 팀 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>배포</x:t>
-  </x:si>
-  <x:si>
-    <x:t>백엔드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디자인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>api</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모델링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>O</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>체크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>원인별 에러 출력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인여부</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀원이 모두 모집되었을 경우, 해당 팀 카드는 메인에서 제외</x:t>
-  </x:si>
-  <x:si>
-    <x:t>페이지 전환 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 페이지 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 페이지 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>나의 프로필 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 팀/사용자 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가 기능 구현</x:t>
-  </x:si>
-  <x:si>
-    <x:t>배포 및 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로세스/태스크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인/회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 사용자 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 등록 해제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지 수정/조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀장 등록 해제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인 페이지 이동(로그인 성공 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/signup/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/accounts/signout/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RESTful url/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인/로그아웃/회원가입/회원탈퇴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 사용자 조회/개별 사용자 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/logout/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체/개별 멤버 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 멤버 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 변경 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 팀 페이지</x:t>
+    <x:t>메인페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그아웃</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 팀 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 탈퇴 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소셜 로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 카드 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 변경</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이팀페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>덤프데이터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구현서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>도착페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 여부</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>footer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유저 본인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 생성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용자 북마크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통합 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원탈퇴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>출발페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>해당 팀 멤버</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/&lt;int: user_pk&gt;/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인이 필요한 서비스입니다 메시지 알림 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>원인별 회원 가입 에러 출력(회원 가입 실패 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개인이 팀에 속하게 될 경우 개인 카드에서 제외</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 로그인 된 상태로 메인페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체/개별 팀 조회</x:t>
   </x:si>
   <x:si>
     <x:t>개별 멤버 페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>전체/개별 팀 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/accounts/&lt;int:user_pk&gt;/mypage/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/accounts/&lt;int: user_pk&gt;/bookmark/</x:t>
+    <x:t>개인 카드 조회</x:t>
   </x:si>
   <x:si>
     <x:t>로그아웃 페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>개인 카드 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/accounts/&lt;int: user_pk&gt;/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인이 필요한 서비스입니다 메시지 알림 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>원인별 회원 가입 에러 출력(회원 가입 실패 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개인이 팀에 속하게 될 경우 개인 카드에서 제외</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 탈퇴 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 찾기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.3.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소셜 로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능명세서</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프론트엔드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그아웃</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 팀 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>check</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.3.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원탈퇴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능구현</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용자 북마크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통합 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 변경</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구현서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/teams/&lt;int: team_pk&gt;/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>원인별 로그인 에러 출력(로그인 실패 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인 페이지 이동(회원 가입 성공 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지 이동(팀 생성 성공 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/password/rest</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지 이동(팀이 있을 경우)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 카드 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 로그아웃 완료 alert창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀장</x:t>
-  </x:si>
-  <x:si>
-    <x:t>조건</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이팀페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>출발페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>덤프데이터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 로그인 된 상태로 메인페이지로 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>도착페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유저 본인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navbar 페이지연결</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 마이 페이지로 이동</x:t>
+    <x:t>북마크 모아보기 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀이 없는 유저</x:t>
   </x:si>
   <x:si>
     <x:t>회원가입 페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>로그인 여부</x:t>
-  </x:si>
-  <x:si>
     <x:t>팀 프로필 수정</x:t>
   </x:si>
   <x:si>
-    <x:t>북마크 모아보기 기능</x:t>
-  </x:si>
-  <x:si>
     <x:t>팀 카드 상세조회</x:t>
   </x:si>
   <x:si>
-    <x:t>성공 시, 메인 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
     <x:t>팀이 있는 유저</x:t>
   </x:si>
   <x:si>
-    <x:t>팀이 없는 유저</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀을 만드는 유저가 팀장이 됨</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인페이지에 유저 추가 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>완료 여부</x:t>
-  </x:si>
-  <x:si>
-    <x:t>footer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>해당 팀 멤버</x:t>
-  </x:si>
-  <x:si>
-    <x:t>드롭다운으로 데이터 출력</x:t>
+    <x:t>반응형..</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -545,7 +548,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="164" formatCode="mm\/dd"/>
   </x:numFmts>
-  <x:fonts count="10">
+  <x:fonts count="11">
     <x:font>
       <x:name val="맑은 고딕"/>
       <x:sz val="11"/>
@@ -598,6 +601,27 @@
       <x:color rgb="ff000000"/>
       <x:b val="1"/>
     </x:font>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ff000000"/>
+          <x:strike val="1"/>
+          <hs:strikeoutShape val="solid"/>
+          <hs:strikeoutType val="1"/>
+          <hs:strikeoutColor rgb="ff000000"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ff000000"/>
+          <x:strike val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:fonts>
   <x:fills count="19">
     <x:fill>
@@ -1051,13 +1075,13 @@
       </x:diagonal>
     </x:border>
     <x:border diagonalUp="1" diagonalDown="1">
-      <x:left style="medium">
+      <x:left style="thin">
         <x:color indexed="64"/>
       </x:left>
-      <x:right style="thin">
+      <x:right style="medium">
         <x:color indexed="64"/>
       </x:right>
-      <x:top>
+      <x:top style="medium">
         <x:color indexed="64"/>
       </x:top>
       <x:bottom style="thin">
@@ -1077,7 +1101,7 @@
       <x:top>
         <x:color indexed="64"/>
       </x:top>
-      <x:bottom style="medium">
+      <x:bottom style="thin">
         <x:color indexed="64"/>
       </x:bottom>
       <x:diagonal>
@@ -1091,10 +1115,10 @@
       <x:right style="thin">
         <x:color indexed="64"/>
       </x:right>
-      <x:top style="medium">
+      <x:top>
         <x:color indexed="64"/>
       </x:top>
-      <x:bottom>
+      <x:bottom style="medium">
         <x:color indexed="64"/>
       </x:bottom>
       <x:diagonal>
@@ -1108,7 +1132,7 @@
       <x:right style="thin">
         <x:color indexed="64"/>
       </x:right>
-      <x:top>
+      <x:top style="medium">
         <x:color indexed="64"/>
       </x:top>
       <x:bottom>
@@ -1119,16 +1143,16 @@
       </x:diagonal>
     </x:border>
     <x:border diagonalUp="1" diagonalDown="1">
-      <x:left style="thin">
+      <x:left style="medium">
         <x:color indexed="64"/>
       </x:left>
-      <x:right style="medium">
+      <x:right style="thin">
         <x:color indexed="64"/>
       </x:right>
-      <x:top style="medium">
+      <x:top>
         <x:color indexed="64"/>
       </x:top>
-      <x:bottom style="thin">
+      <x:bottom>
         <x:color indexed="64"/>
       </x:bottom>
       <x:diagonal>
@@ -1183,7 +1207,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="115">
+  <x:cellXfs count="117">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -1658,6 +1682,123 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -1671,13 +1812,13 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1710,13 +1851,13 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1736,26 +1877,13 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1775,13 +1903,26 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1801,26 +1942,26 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1840,26 +1981,26 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1879,26 +2020,26 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1918,26 +2059,26 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -1957,104 +2098,13 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+        <x:xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -2796,34 +2846,34 @@
     <x:row r="2" spans="2:14">
       <x:c r="B2" s="4"/>
       <x:c r="C2" s="5"/>
-      <x:c r="D2" s="110"/>
-      <x:c r="E2" s="110"/>
-      <x:c r="F2" s="110"/>
-      <x:c r="G2" s="110"/>
-      <x:c r="H2" s="110"/>
-      <x:c r="I2" s="110"/>
-      <x:c r="J2" s="110"/>
-      <x:c r="K2" s="110"/>
-      <x:c r="L2" s="110"/>
-      <x:c r="M2" s="110"/>
-      <x:c r="N2" s="111"/>
+      <x:c r="D2" s="91"/>
+      <x:c r="E2" s="91"/>
+      <x:c r="F2" s="91"/>
+      <x:c r="G2" s="91"/>
+      <x:c r="H2" s="91"/>
+      <x:c r="I2" s="91"/>
+      <x:c r="J2" s="91"/>
+      <x:c r="K2" s="91"/>
+      <x:c r="L2" s="91"/>
+      <x:c r="M2" s="91"/>
+      <x:c r="N2" s="92"/>
     </x:row>
     <x:row r="3" spans="2:14">
       <x:c r="B3" s="6"/>
       <x:c r="C3" s="3"/>
-      <x:c r="D3" s="108"/>
-      <x:c r="E3" s="108"/>
-      <x:c r="F3" s="108"/>
-      <x:c r="G3" s="108"/>
-      <x:c r="H3" s="108" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="I3" s="108"/>
-      <x:c r="J3" s="108"/>
-      <x:c r="K3" s="108"/>
-      <x:c r="L3" s="108"/>
-      <x:c r="M3" s="108"/>
-      <x:c r="N3" s="109"/>
+      <x:c r="D3" s="89"/>
+      <x:c r="E3" s="89"/>
+      <x:c r="F3" s="89"/>
+      <x:c r="G3" s="89"/>
+      <x:c r="H3" s="89" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="I3" s="89"/>
+      <x:c r="J3" s="89"/>
+      <x:c r="K3" s="89"/>
+      <x:c r="L3" s="89"/>
+      <x:c r="M3" s="89"/>
+      <x:c r="N3" s="90"/>
     </x:row>
     <x:row r="4" spans="2:14">
       <x:c r="B4" s="6"/>
@@ -2864,10 +2914,10 @@
     </x:row>
     <x:row r="5" spans="2:14">
       <x:c r="B5" s="6" t="s">
-        <x:v>51</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
-        <x:v>69</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D5" s="3"/>
       <x:c r="E5" s="3"/>
@@ -2883,10 +2933,10 @@
     </x:row>
     <x:row r="6" spans="2:14">
       <x:c r="B6" s="25" t="s">
-        <x:v>29</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
-        <x:v>32</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D6" s="36"/>
       <x:c r="E6" s="16"/>
@@ -2902,10 +2952,10 @@
     </x:row>
     <x:row r="7" spans="2:14">
       <x:c r="B7" s="12" t="s">
-        <x:v>48</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D7" s="9"/>
       <x:c r="E7" s="16"/>
@@ -2921,10 +2971,10 @@
     </x:row>
     <x:row r="8" spans="2:14">
       <x:c r="B8" s="12" t="s">
-        <x:v>37</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>81</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D8" s="9"/>
       <x:c r="E8" s="16"/>
@@ -2940,10 +2990,10 @@
     </x:row>
     <x:row r="9" spans="2:14">
       <x:c r="B9" s="12" t="s">
-        <x:v>105</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D9" s="9"/>
       <x:c r="E9" s="16"/>
@@ -2959,10 +3009,10 @@
     </x:row>
     <x:row r="10" spans="2:14">
       <x:c r="B10" s="12" t="s">
-        <x:v>115</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D10" s="9"/>
       <x:c r="E10" s="16"/>
@@ -2979,7 +3029,7 @@
     <x:row r="11" spans="2:14">
       <x:c r="B11" s="12"/>
       <x:c r="C11" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D11" s="9"/>
       <x:c r="E11" s="16"/>
@@ -2996,7 +3046,7 @@
     <x:row r="12" spans="2:14">
       <x:c r="B12" s="12"/>
       <x:c r="C12" s="3" t="s">
-        <x:v>83</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D12" s="9"/>
       <x:c r="E12" s="16"/>
@@ -3013,7 +3063,7 @@
     <x:row r="13" spans="2:14">
       <x:c r="B13" s="12"/>
       <x:c r="C13" s="3" t="s">
-        <x:v>75</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D13" s="9"/>
       <x:c r="E13" s="16"/>
@@ -3030,7 +3080,7 @@
     <x:row r="14" spans="2:14">
       <x:c r="B14" s="12"/>
       <x:c r="C14" s="3" t="s">
-        <x:v>77</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D14" s="9"/>
       <x:c r="E14" s="16"/>
@@ -3061,10 +3111,10 @@
     </x:row>
     <x:row r="16" spans="2:14">
       <x:c r="B16" s="26" t="s">
-        <x:v>56</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C16" s="10" t="s">
-        <x:v>109</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="D16" s="16"/>
       <x:c r="E16" s="37"/>
@@ -3080,10 +3130,10 @@
     </x:row>
     <x:row r="17" spans="2:14">
       <x:c r="B17" s="12" t="s">
-        <x:v>57</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C17" s="3" t="s">
-        <x:v>121</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D17" s="16"/>
       <x:c r="E17" s="10"/>
@@ -3099,10 +3149,10 @@
     </x:row>
     <x:row r="18" spans="2:14">
       <x:c r="B18" s="12" t="s">
-        <x:v>116</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C18" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D18" s="16"/>
       <x:c r="E18" s="10"/>
@@ -3118,10 +3168,10 @@
     </x:row>
     <x:row r="19" spans="2:14">
       <x:c r="B19" s="12" t="s">
-        <x:v>119</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="C19" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D19" s="16"/>
       <x:c r="E19" s="10"/>
@@ -3137,10 +3187,10 @@
     </x:row>
     <x:row r="20" spans="2:14">
       <x:c r="B20" s="12" t="s">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C20" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D20" s="16"/>
       <x:c r="E20" s="10"/>
@@ -3156,10 +3206,10 @@
     </x:row>
     <x:row r="21" spans="2:14">
       <x:c r="B21" s="12" t="s">
-        <x:v>126</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C21" s="3" t="s">
-        <x:v>83</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D21" s="16"/>
       <x:c r="E21" s="10"/>
@@ -3175,10 +3225,10 @@
     </x:row>
     <x:row r="22" spans="2:14">
       <x:c r="B22" s="12" t="s">
-        <x:v>129</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="C22" s="3" t="s">
-        <x:v>75</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D22" s="16"/>
       <x:c r="E22" s="10"/>
@@ -3194,10 +3244,10 @@
     </x:row>
     <x:row r="23" spans="2:14">
       <x:c r="B23" s="12" t="s">
-        <x:v>128</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C23" s="3" t="s">
-        <x:v>77</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D23" s="16"/>
       <x:c r="E23" s="10"/>
@@ -3213,10 +3263,10 @@
     </x:row>
     <x:row r="24" spans="2:14">
       <x:c r="B24" s="12" t="s">
-        <x:v>34</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C24" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D24" s="16"/>
       <x:c r="E24" s="16"/>
@@ -3232,7 +3282,7 @@
     </x:row>
     <x:row r="25" spans="2:14">
       <x:c r="B25" s="12" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C25" s="3" t="s">
         <x:v>130</x:v>
@@ -3251,10 +3301,10 @@
     </x:row>
     <x:row r="26" spans="2:14">
       <x:c r="B26" s="12" t="s">
-        <x:v>123</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C26" s="3" t="s">
-        <x:v>120</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D26" s="16"/>
       <x:c r="E26" s="16"/>
@@ -3270,10 +3320,10 @@
     </x:row>
     <x:row r="27" spans="2:14">
       <x:c r="B27" s="12" t="s">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C27" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D27" s="16"/>
       <x:c r="E27" s="16"/>
@@ -3289,10 +3339,10 @@
     </x:row>
     <x:row r="28" spans="2:14">
       <x:c r="B28" s="12" t="s">
-        <x:v>134</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="C28" s="3" t="s">
-        <x:v>135</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D28" s="16"/>
       <x:c r="E28" s="16"/>
@@ -3323,10 +3373,10 @@
     </x:row>
     <x:row r="30" spans="2:14">
       <x:c r="B30" s="29" t="s">
-        <x:v>33</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C30" s="11" t="s">
-        <x:v>67</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D30" s="16"/>
       <x:c r="E30" s="16"/>
@@ -3342,10 +3392,10 @@
     </x:row>
     <x:row r="31" spans="2:14">
       <x:c r="B31" s="12" t="s">
-        <x:v>35</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C31" s="3" t="s">
-        <x:v>107</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="D31" s="16"/>
       <x:c r="E31" s="16"/>
@@ -3361,10 +3411,10 @@
     </x:row>
     <x:row r="32" spans="2:14">
       <x:c r="B32" s="12" t="s">
-        <x:v>44</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C32" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D32" s="16"/>
       <x:c r="E32" s="16"/>
@@ -3395,10 +3445,10 @@
     </x:row>
     <x:row r="34" spans="2:14">
       <x:c r="B34" s="27" t="s">
-        <x:v>45</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C34" s="28" t="s">
-        <x:v>124</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D34" s="16"/>
       <x:c r="E34" s="16"/>
@@ -3414,10 +3464,10 @@
     </x:row>
     <x:row r="35" spans="2:14">
       <x:c r="B35" s="12" t="s">
-        <x:v>50</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C35" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D35" s="16"/>
       <x:c r="E35" s="16"/>
@@ -3448,10 +3498,10 @@
     </x:row>
     <x:row r="37" spans="2:14">
       <x:c r="B37" s="30" t="s">
-        <x:v>38</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C37" s="31" t="s">
-        <x:v>31</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D37" s="16"/>
       <x:c r="E37" s="16"/>
@@ -3467,10 +3517,10 @@
     </x:row>
     <x:row r="38" spans="2:14" ht="18">
       <x:c r="B38" s="13" t="s">
-        <x:v>39</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C38" s="8" t="s">
-        <x:v>68</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D38" s="24"/>
       <x:c r="E38" s="24"/>
@@ -3496,7 +3546,7 @@
     <x:mergeCell ref="H3:N3"/>
     <x:mergeCell ref="D2:N2"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -3530,85 +3580,85 @@
     <x:row r="3" ht="18"/>
     <x:row r="4" spans="2:6">
       <x:c r="B4" s="45" t="s">
-        <x:v>41</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C4" s="44" t="s">
-        <x:v>43</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D4" s="44" t="s">
-        <x:v>46</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E4" s="47" t="s">
-        <x:v>114</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F4" s="17"/>
     </x:row>
     <x:row r="5" spans="2:6">
       <x:c r="B5" s="18" t="s">
-        <x:v>113</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>113</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="D5" s="16" t="s">
-        <x:v>30</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E5" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F5" s="20"/>
     </x:row>
     <x:row r="6" spans="2:6">
       <x:c r="B6" s="6" t="s">
-        <x:v>70</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E6" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F6" s="43"/>
     </x:row>
     <x:row r="7" spans="2:6">
       <x:c r="B7" s="6"/>
       <x:c r="C7" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E7" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F7" s="43"/>
     </x:row>
     <x:row r="8" spans="2:6">
       <x:c r="B8" s="6"/>
       <x:c r="C8" s="3" t="s">
-        <x:v>111</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
-        <x:v>84</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E8" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F8" s="43"/>
     </x:row>
     <x:row r="9" spans="2:6">
       <x:c r="B9" s="6"/>
       <x:c r="C9" s="3" t="s">
-        <x:v>103</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
-        <x:v>141</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E9" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F9" s="43"/>
     </x:row>
@@ -3621,39 +3671,39 @@
     </x:row>
     <x:row r="11" spans="2:6">
       <x:c r="B11" s="6" t="s">
-        <x:v>118</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E11" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F11" s="43"/>
     </x:row>
     <x:row r="12" spans="2:6">
       <x:c r="B12" s="6"/>
       <x:c r="C12" s="3" t="s">
-        <x:v>73</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D12" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E12" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F12" s="43"/>
     </x:row>
     <x:row r="13" spans="2:6">
       <x:c r="B13" s="6"/>
       <x:c r="C13" s="3" t="s">
-        <x:v>117</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D13" s="3" t="s">
-        <x:v>80</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E13" s="42"/>
       <x:c r="F13" s="43"/>
@@ -3667,55 +3717,55 @@
     </x:row>
     <x:row r="15" spans="2:6">
       <x:c r="B15" s="32" t="s">
-        <x:v>120</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C15" s="33" t="s">
-        <x:v>66</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D15" s="33" t="s">
-        <x:v>30</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E15" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F15" s="35"/>
     </x:row>
     <x:row r="16" spans="2:6">
       <x:c r="B16" s="32"/>
       <x:c r="C16" s="33" t="s">
-        <x:v>65</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D16" s="33" t="s">
-        <x:v>12</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="E16" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F16" s="35"/>
     </x:row>
     <x:row r="17" spans="2:6">
       <x:c r="B17" s="32"/>
       <x:c r="C17" s="33" t="s">
-        <x:v>72</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D17" s="33" t="s">
-        <x:v>98</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="E17" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F17" s="35"/>
     </x:row>
     <x:row r="18" spans="2:6">
       <x:c r="B18" s="32"/>
       <x:c r="C18" s="33" t="s">
-        <x:v>122</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="D18" s="33" t="s">
-        <x:v>95</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E18" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F18" s="35"/>
     </x:row>
@@ -3728,29 +3778,29 @@
     </x:row>
     <x:row r="20" spans="2:6">
       <x:c r="B20" s="32" t="s">
-        <x:v>74</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C20" s="33" t="s">
-        <x:v>112</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="D20" s="33" t="s">
-        <x:v>137</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E20" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F20" s="35"/>
     </x:row>
     <x:row r="21" spans="2:6">
       <x:c r="B21" s="32"/>
       <x:c r="C21" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D21" s="46" t="s">
-        <x:v>16</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E21" s="42" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="F21" s="35"/>
     </x:row>
@@ -3762,7 +3812,7 @@
       <x:c r="F22" s="22"/>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -3788,344 +3838,344 @@
     <x:row r="1" ht="9" customHeight="1"/>
     <x:row r="2" spans="2:2" ht="17.800000000000001">
       <x:c r="B2" s="83" t="s">
-        <x:v>133</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="3" ht="9" customHeight="1"/>
     <x:row r="4" spans="2:5" ht="18.550000000000001">
       <x:c r="B4" s="50" t="s">
-        <x:v>41</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C4" s="51" t="s">
-        <x:v>54</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="D4" s="51" t="s">
-        <x:v>9</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E4" s="52" t="s">
-        <x:v>52</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="48"/>
-      <x:c r="B5" s="91" t="s">
-        <x:v>120</x:v>
+      <x:c r="B5" s="100" t="s">
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C5" s="61" t="s">
-        <x:v>63</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D5" s="54"/>
       <x:c r="E5" s="64" t="s">
-        <x:v>99</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="48"/>
-      <x:c r="B6" s="92"/>
+      <x:c r="B6" s="101"/>
       <x:c r="C6" s="62" t="s">
-        <x:v>111</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D6" s="55" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E6" s="63" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="48"/>
-      <x:c r="B7" s="92"/>
+      <x:c r="B7" s="101"/>
       <x:c r="C7" s="62" t="s">
-        <x:v>64</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D7" s="55" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E7" s="63" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="48"/>
-      <x:c r="B8" s="92"/>
+      <x:c r="B8" s="101"/>
       <x:c r="C8" s="62" t="s">
-        <x:v>10</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="D8" s="55" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E8" s="63" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="48"/>
-      <x:c r="B9" s="92"/>
+      <x:c r="B9" s="101"/>
       <x:c r="C9" s="62" t="s">
-        <x:v>142</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D9" s="55" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E9" s="63" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="48"/>
-      <x:c r="B10" s="92"/>
+      <x:c r="B10" s="101"/>
       <x:c r="C10" s="62" t="s">
-        <x:v>93</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D10" s="55"/>
       <x:c r="E10" s="65"/>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="48"/>
-      <x:c r="B11" s="92"/>
+      <x:c r="B11" s="101"/>
       <x:c r="C11" s="62" t="s">
-        <x:v>85</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D11" s="55"/>
       <x:c r="E11" s="65"/>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="48"/>
-      <x:c r="B12" s="93"/>
+      <x:c r="B12" s="102"/>
       <x:c r="C12" s="62"/>
       <x:c r="D12" s="55"/>
       <x:c r="E12" s="65"/>
     </x:row>
     <x:row r="13" spans="2:5">
-      <x:c r="B13" s="94" t="s">
+      <x:c r="B13" s="103" t="s">
         <x:v>130</x:v>
       </x:c>
       <x:c r="C13" s="56" t="s">
-        <x:v>18</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="D13" s="56"/>
       <x:c r="E13" s="73" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5">
-      <x:c r="B14" s="95"/>
+      <x:c r="B14" s="104"/>
       <x:c r="C14" s="56" t="s">
-        <x:v>78</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D14" s="56"/>
       <x:c r="E14" s="73" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5">
-      <x:c r="B15" s="95"/>
+      <x:c r="B15" s="104"/>
       <x:c r="C15" s="56" t="s">
-        <x:v>138</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D15" s="56"/>
       <x:c r="E15" s="66"/>
     </x:row>
     <x:row r="16" spans="2:5">
-      <x:c r="B16" s="96"/>
+      <x:c r="B16" s="105"/>
       <x:c r="C16" s="56"/>
       <x:c r="D16" s="56"/>
       <x:c r="E16" s="66"/>
     </x:row>
     <x:row r="17" spans="2:5">
-      <x:c r="B17" s="97" t="s">
-        <x:v>88</x:v>
+      <x:c r="B17" s="106" t="s">
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C17" s="57" t="s">
-        <x:v>139</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D17" s="57"/>
       <x:c r="E17" s="74" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5">
-      <x:c r="B18" s="98"/>
+      <x:c r="B18" s="107"/>
       <x:c r="C18" s="57" t="s">
-        <x:v>100</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D18" s="57"/>
       <x:c r="E18" s="67"/>
     </x:row>
     <x:row r="19" spans="2:5">
-      <x:c r="B19" s="99"/>
+      <x:c r="B19" s="108"/>
       <x:c r="C19" s="57"/>
       <x:c r="D19" s="57"/>
       <x:c r="E19" s="67"/>
     </x:row>
     <x:row r="20" spans="2:5">
-      <x:c r="B20" s="100" t="s">
-        <x:v>132</x:v>
+      <x:c r="B20" s="109" t="s">
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C20" s="60" t="s">
-        <x:v>65</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D20" s="60" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E20" s="75" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="2:5">
-      <x:c r="B21" s="101"/>
+      <x:c r="B21" s="110"/>
       <x:c r="C21" s="60" t="s">
-        <x:v>8</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D21" s="60" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E21" s="68"/>
     </x:row>
     <x:row r="22" spans="2:5">
-      <x:c r="B22" s="101"/>
+      <x:c r="B22" s="110"/>
       <x:c r="C22" s="60" t="s">
-        <x:v>13</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D22" s="60" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E22" s="68"/>
     </x:row>
     <x:row r="23" spans="2:5">
-      <x:c r="B23" s="102"/>
+      <x:c r="B23" s="111"/>
       <x:c r="C23" s="60"/>
       <x:c r="D23" s="60"/>
       <x:c r="E23" s="68"/>
     </x:row>
     <x:row r="24" spans="2:5">
-      <x:c r="B24" s="103" t="s">
-        <x:v>87</x:v>
+      <x:c r="B24" s="112" t="s">
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C24" s="59" t="s">
-        <x:v>131</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D24" s="59" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E24" s="69"/>
     </x:row>
     <x:row r="25" spans="2:5">
-      <x:c r="B25" s="104"/>
+      <x:c r="B25" s="113"/>
       <x:c r="C25" s="59" t="s">
-        <x:v>19</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D25" s="59" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E25" s="69"/>
     </x:row>
     <x:row r="26" spans="2:5">
-      <x:c r="B26" s="105"/>
+      <x:c r="B26" s="114"/>
       <x:c r="C26" s="59"/>
       <x:c r="D26" s="59"/>
       <x:c r="E26" s="69"/>
     </x:row>
     <x:row r="27" spans="2:5">
-      <x:c r="B27" s="106" t="s">
-        <x:v>89</x:v>
+      <x:c r="B27" s="115" t="s">
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C27" s="53" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="D27" s="53" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E27" s="70"/>
     </x:row>
     <x:row r="28" spans="2:5">
-      <x:c r="B28" s="107"/>
+      <x:c r="B28" s="116"/>
       <x:c r="C28" s="53"/>
       <x:c r="D28" s="53"/>
       <x:c r="E28" s="70"/>
     </x:row>
     <x:row r="29" spans="2:5">
-      <x:c r="B29" s="84" t="s">
-        <x:v>74</x:v>
+      <x:c r="B29" s="93" t="s">
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C29" s="58" t="s">
-        <x:v>14</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D29" s="58" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E29" s="71"/>
     </x:row>
     <x:row r="30" spans="2:5">
-      <x:c r="B30" s="85"/>
+      <x:c r="B30" s="94"/>
       <x:c r="C30" s="58"/>
       <x:c r="D30" s="58"/>
       <x:c r="E30" s="71"/>
     </x:row>
     <x:row r="31" spans="2:5">
-      <x:c r="B31" s="86" t="s">
-        <x:v>90</x:v>
+      <x:c r="B31" s="95" t="s">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C31" s="49" t="s">
-        <x:v>136</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D31" s="49" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E31" s="76" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="2:5">
-      <x:c r="B32" s="86"/>
+      <x:c r="B32" s="95"/>
       <x:c r="C32" s="49" t="s">
-        <x:v>140</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D32" s="49" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E32" s="76" t="s">
-        <x:v>49</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="2:5">
-      <x:c r="B33" s="86"/>
+      <x:c r="B33" s="95"/>
       <x:c r="C33" s="49"/>
       <x:c r="D33" s="49"/>
       <x:c r="E33" s="72"/>
     </x:row>
     <x:row r="34" spans="2:5">
-      <x:c r="B34" s="87" t="s">
-        <x:v>91</x:v>
+      <x:c r="B34" s="96" t="s">
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C34" s="81" t="s">
-        <x:v>112</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="D34" s="81"/>
       <x:c r="E34" s="82" t="s">
-        <x:v>15</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="2:5">
-      <x:c r="B35" s="88"/>
+      <x:c r="B35" s="97"/>
       <x:c r="C35" s="81"/>
       <x:c r="D35" s="81"/>
       <x:c r="E35" s="82"/>
     </x:row>
     <x:row r="36" spans="2:5">
-      <x:c r="B36" s="89" t="s">
-        <x:v>92</x:v>
+      <x:c r="B36" s="98" t="s">
+        <x:v>164</x:v>
       </x:c>
       <x:c r="C36" s="77" t="s">
-        <x:v>86</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D36" s="77"/>
       <x:c r="E36" s="78"/>
     </x:row>
     <x:row r="37" spans="2:5" ht="16.75">
-      <x:c r="B37" s="90"/>
+      <x:c r="B37" s="99"/>
       <x:c r="C37" s="79" t="s">
-        <x:v>53</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D37" s="79"/>
       <x:c r="E37" s="80"/>
@@ -4143,7 +4193,7 @@
     <x:mergeCell ref="B24:B26"/>
     <x:mergeCell ref="B27:B28"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -4153,638 +4203,643 @@
   <x:sheetPr codeName="Sheet4"/>
   <x:dimension ref="B2:J49"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="H21" activeCellId="0" sqref="H21:H21"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="C8" activeCellId="0" sqref="C8:C8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="1" max="1" width="3.125" style="112" customWidth="1"/>
-    <x:col min="2" max="2" width="9.00390625" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="16.95703125" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="15.1875" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="5" width="17.09765625" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="41.63671875" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="7" max="7" width="52.140625" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="8" max="9" width="39.484375" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="10" max="10" width="28.34765625" style="112" bestFit="1" customWidth="1"/>
-    <x:col min="11" max="16384" width="9.00390625" style="112"/>
+    <x:col min="1" max="1" width="3.125" style="84" customWidth="1"/>
+    <x:col min="2" max="2" width="9.00390625" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="16.95703125" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="15.1875" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="17.09765625" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="41.63671875" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="7" max="7" width="52.140625" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="8" max="9" width="39.484375" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="10" max="10" width="28.34765625" style="84" bestFit="1" customWidth="1"/>
+    <x:col min="11" max="16384" width="9.00390625" style="84"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="2:4">
-      <x:c r="B2" s="112" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C2" s="112" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="D2" s="112" t="s">
+    <x:row r="2" spans="2:3">
+      <x:c r="B2" s="84" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C2" s="84" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="2:3">
+      <x:c r="B3" s="84">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="86" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="2:3">
+      <x:c r="B4" s="84">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C4" s="86" t="s">
+        <x:v>138</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="2:3">
+      <x:c r="B5" s="84">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C5" s="86" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="2:4">
+      <x:c r="B6" s="84">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C6" s="87" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="D6" s="84" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="2:3">
+      <x:c r="B7" s="84">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C7" s="86" t="s">
+        <x:v>114</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="2:3">
+      <x:c r="B8" s="84">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C8" s="84" t="s">
         <x:v>169</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="2:3">
-      <x:c r="B3" s="112">
+    <x:row r="9" spans="2:3">
+      <x:c r="B9" s="84">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C9" s="84" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="2:3">
+      <x:c r="B10" s="84">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C10" s="84" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="2:3">
+      <x:c r="B11" s="84">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C11" s="84" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="2:3">
+      <x:c r="B12" s="84">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C12" s="84" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="2:3">
+      <x:c r="B13" s="84">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C13" s="84" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="2:3">
+      <x:c r="B14" s="84">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C14" s="84" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="2:3">
+      <x:c r="B15" s="84">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C15" s="84" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="2:6" ht="17.800000000000001">
+      <x:c r="B18" s="88" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C18" s="88"/>
+      <x:c r="D18" s="88"/>
+      <x:c r="E18" s="88"/>
+      <x:c r="F18" s="88"/>
+    </x:row>
+    <x:row r="19" spans="2:7">
+      <x:c r="B19" s="84" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C19" s="84" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="D19" s="84" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="E19" s="85" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="F19" s="85" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="G19" s="84" t="s">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="2:7">
+      <x:c r="B20" s="84">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="112" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="2:3">
-      <x:c r="B4" s="112">
+      <x:c r="C20" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E20" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="G20" s="84" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="2:6">
+      <x:c r="B21" s="84">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C4" s="112" t="s">
+      <x:c r="C21" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E21" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F21" s="84" t="s">
+        <x:v>130</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="2:6">
+      <x:c r="B22" s="84">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C22" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E22" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F22" s="84" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="2:6">
+      <x:c r="B23" s="84">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C23" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E23" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F23" s="84" t="s">
+        <x:v>126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="2:6">
+      <x:c r="B24" s="84">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C24" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E24" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F24" s="84" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="2:6">
+      <x:c r="B25" s="84">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C25" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D25" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E25" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F25" s="84" t="s">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="2:6">
+      <x:c r="B26" s="84">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C26" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D26" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E26" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F26" s="84" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="2:6">
+      <x:c r="B27" s="84">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C27" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D27" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E27" s="84" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="F27" s="84" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="2:6">
+      <x:c r="B28" s="84">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C28" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D28" s="84" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="E28" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F28" s="84" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="2:6">
+      <x:c r="B29" s="84">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C29" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D29" s="84" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E29" s="84" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="F29" s="84" t="s">
+        <x:v>98</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="2:6">
+      <x:c r="B30" s="84">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C30" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D30" s="84" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="E30" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F30" s="84" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="2:6">
+      <x:c r="B31" s="84">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C31" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E31" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F31" s="84" t="s">
+        <x:v>126</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="2:6">
+      <x:c r="B32" s="84">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C32" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E32" s="84" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F32" s="84" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="2:6" ht="17.800000000000001">
+      <x:c r="B35" s="88" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="C35" s="88"/>
+      <x:c r="D35" s="88"/>
+      <x:c r="E35" s="88"/>
+      <x:c r="F35" s="88"/>
+    </x:row>
+    <x:row r="36" spans="2:10">
+      <x:c r="B36" s="84" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C36" s="84" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="D36" s="84" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="E36" s="84" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="F36" s="84" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="G36" s="84" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="H36" s="84" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="I36" s="84" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="J36" s="84" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="2:7">
+      <x:c r="B37" s="84">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C37" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D37" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E37" s="84" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F37" s="87" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G37" s="84" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="2:7">
+      <x:c r="B38" s="84">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C38" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D38" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E38" s="84" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="F38" s="84" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G38" s="84" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="2:10">
+      <x:c r="B39" s="84">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C39" s="84" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E39" s="84" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="F39" s="84" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G39" s="84" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H39" s="84" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="I39" s="84" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="J39" s="84" t="s">
+        <x:v>95</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="2:7">
+      <x:c r="B40" s="84">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C40" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D40" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E40" s="84" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F40" s="84" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G40" s="84" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="2:10">
+      <x:c r="B41" s="84">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C41" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D41" s="84" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="E41" s="84" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="F41" s="84" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G41" s="84" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H41" s="84" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="I41" s="84" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="J41" s="84" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="2:8">
+      <x:c r="B42" s="84">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C42" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D42" s="84" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E42" s="84" t="s">
         <x:v>170</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="2:4">
-      <x:c r="B5" s="112">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C5" s="112" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D5" s="112" t="s">
+      <x:c r="F42" s="84" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G42" s="84" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H42" s="84" t="s">
         <x:v>49</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="2:3">
-      <x:c r="B6" s="112">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C6" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="2:3">
-      <x:c r="B7" s="112">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C7" s="112" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="2:3">
-      <x:c r="B8" s="112">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C8" s="112" t="s">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="2:3">
-      <x:c r="B9" s="112">
+    <x:row r="43" spans="2:6">
+      <x:c r="B43" s="84">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C9" s="112" t="s">
-        <x:v>163</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="2:3">
-      <x:c r="B10" s="112">
+      <x:c r="C43" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D43" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E43" s="84" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="F43" s="84" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="2:7">
+      <x:c r="B44" s="84">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C10" s="112" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="2:3">
-      <x:c r="B11" s="112">
+      <x:c r="C44" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D44" s="84" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="E44" s="84" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="F44" s="84" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G44" s="84" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="2:7">
+      <x:c r="B45" s="84">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C11" s="112" t="s">
-        <x:v>118</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="2:3">
-      <x:c r="B12" s="112">
+      <x:c r="C45" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E45" s="84" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="F45" s="84" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="G45" s="84" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="2:6">
+      <x:c r="B46" s="84">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C12" s="112" t="s">
+      <x:c r="C46" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D46" s="84" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="E46" s="84" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F46" s="84" t="s">
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="2:6">
+      <x:c r="B47" s="84">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C47" s="84" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E47" s="84" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="F47" s="84" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="2:5">
+      <x:c r="B48" s="84">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E48" s="84" t="s">
+        <x:v>99</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="2:5">
+      <x:c r="B49" s="84">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E49" s="84" t="s">
         <x:v>131</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="2:3">
-      <x:c r="B13" s="112">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C13" s="112" t="s">
-        <x:v>74</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="2:3">
-      <x:c r="B14" s="112">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C14" s="112" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="2:6" ht="17.800000000000001">
-      <x:c r="B18" s="113" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C18" s="113"/>
-      <x:c r="D18" s="113"/>
-      <x:c r="E18" s="113"/>
-      <x:c r="F18" s="113"/>
-    </x:row>
-    <x:row r="19" spans="2:7">
-      <x:c r="B19" s="112" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C19" s="112" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="D19" s="112" t="s">
-        <x:v>148</x:v>
-      </x:c>
-      <x:c r="E19" s="114" t="s">
-        <x:v>151</x:v>
-      </x:c>
-      <x:c r="F19" s="114" t="s">
-        <x:v>155</x:v>
-      </x:c>
-      <x:c r="G19" s="112" t="s">
-        <x:v>55</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="2:7">
-      <x:c r="B20" s="112">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C20" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E20" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="G20" s="112" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="2:6">
-      <x:c r="B21" s="112">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C21" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E21" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F21" s="112" t="s">
-        <x:v>130</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="2:6">
-      <x:c r="B22" s="112">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C22" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E22" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F22" s="112" t="s">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="2:6">
-      <x:c r="B23" s="112">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C23" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E23" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F23" s="112" t="s">
-        <x:v>145</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="2:6">
-      <x:c r="B24" s="112">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C24" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E24" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F24" s="112" t="s">
-        <x:v>97</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="2:6">
-      <x:c r="B25" s="112">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C25" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D25" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E25" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F25" s="112" t="s">
-        <x:v>96</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="2:6">
-      <x:c r="B26" s="112">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C26" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D26" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E26" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F26" s="112" t="s">
-        <x:v>118</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="2:6">
-      <x:c r="B27" s="112">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C27" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D27" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E27" s="112" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="F27" s="112" t="s">
-        <x:v>131</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="2:6">
-      <x:c r="B28" s="112">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C28" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D28" s="112" t="s">
-        <x:v>165</x:v>
-      </x:c>
-      <x:c r="E28" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F28" s="112" t="s">
-        <x:v>149</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="2:6">
-      <x:c r="B29" s="112">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C29" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D29" s="112" t="s">
-        <x:v>147</x:v>
-      </x:c>
-      <x:c r="E29" s="112" t="s">
-        <x:v>149</x:v>
-      </x:c>
-      <x:c r="F29" s="112" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="2:6">
-      <x:c r="B30" s="112">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C30" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D30" s="112" t="s">
-        <x:v>166</x:v>
-      </x:c>
-      <x:c r="E30" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F30" s="112" t="s">
-        <x:v>90</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="2:6">
-      <x:c r="B31" s="112">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C31" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E31" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F31" s="112" t="s">
-        <x:v>145</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="2:6">
-      <x:c r="B32" s="112">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C32" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E32" s="112" t="s">
-        <x:v>113</x:v>
-      </x:c>
-      <x:c r="F32" s="112" t="s">
-        <x:v>97</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="2:6" ht="17.800000000000001">
-      <x:c r="B35" s="113" t="s">
-        <x:v>153</x:v>
-      </x:c>
-      <x:c r="C35" s="113"/>
-      <x:c r="D35" s="113"/>
-      <x:c r="E35" s="113"/>
-      <x:c r="F35" s="113"/>
-    </x:row>
-    <x:row r="36" spans="2:10">
-      <x:c r="B36" s="112" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C36" s="112" t="s">
-        <x:v>160</x:v>
-      </x:c>
-      <x:c r="D36" s="112" t="s">
-        <x:v>148</x:v>
-      </x:c>
-      <x:c r="E36" s="112" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F36" s="112" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="G36" s="112" t="s">
-        <x:v>144</x:v>
-      </x:c>
-      <x:c r="H36" s="112" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="I36" s="112" t="s">
-        <x:v>143</x:v>
-      </x:c>
-      <x:c r="J36" s="112" t="s">
-        <x:v>150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="2:7">
-      <x:c r="B37" s="112">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C37" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D37" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E37" s="112" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="F37" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="G37" s="112" t="s">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="2:7">
-      <x:c r="B38" s="112">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C38" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D38" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E38" s="112" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="F38" s="112" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="G38" s="112" t="s">
-        <x:v>164</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="2:10">
-      <x:c r="B39" s="112">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C39" s="112" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E39" s="112" t="s">
-        <x:v>110</x:v>
-      </x:c>
-      <x:c r="F39" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="G39" s="112" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="H39" s="112" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="I39" s="112" t="s">
-        <x:v>168</x:v>
-      </x:c>
-      <x:c r="J39" s="112" t="s">
-        <x:v>172</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="2:7">
-      <x:c r="B40" s="112">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C40" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D40" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E40" s="112" t="s">
-        <x:v>127</x:v>
-      </x:c>
-      <x:c r="F40" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="G40" s="112" t="s">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="2:10">
-      <x:c r="B41" s="112">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C41" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D41" s="112" t="s">
-        <x:v>166</x:v>
-      </x:c>
-      <x:c r="E41" s="112" t="s">
-        <x:v>136</x:v>
-      </x:c>
-      <x:c r="F41" s="112" t="s">
-        <x:v>167</x:v>
-      </x:c>
-      <x:c r="G41" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="H41" s="112" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="I41" s="112" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="J41" s="112" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="2:8">
-      <x:c r="B42" s="112">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C42" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D42" s="112" t="s">
-        <x:v>147</x:v>
-      </x:c>
-      <x:c r="E42" s="112" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="F42" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="G42" s="112" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="H42" s="112" t="s">
-        <x:v>28</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="2:6">
-      <x:c r="B43" s="112">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C43" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D43" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E43" s="112" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="F43" s="112" t="s">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="2:7">
-      <x:c r="B44" s="112">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C44" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D44" s="112" t="s">
-        <x:v>156</x:v>
-      </x:c>
-      <x:c r="E44" s="112" t="s">
-        <x:v>131</x:v>
-      </x:c>
-      <x:c r="F44" s="112" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="G44" s="112" t="s">
-        <x:v>158</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45" spans="2:7">
-      <x:c r="B45" s="112">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C45" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E45" s="112" t="s">
-        <x:v>145</x:v>
-      </x:c>
-      <x:c r="F45" s="112" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G45" s="112" t="s">
-        <x:v>61</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="46" spans="2:6">
-      <x:c r="B46" s="112">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C46" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="D46" s="112" t="s">
-        <x:v>171</x:v>
-      </x:c>
-      <x:c r="E46" s="112" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="F46" s="112" t="s">
-        <x:v>102</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47" spans="2:6">
-      <x:c r="B47" s="112">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C47" s="112" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E47" s="112" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="F47" s="112" t="s">
-        <x:v>101</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="48" spans="2:5">
-      <x:c r="B48" s="112">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E48" s="112" t="s">
-        <x:v>157</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="49" spans="2:5">
-      <x:c r="B49" s="112">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E49" s="112" t="s">
-        <x:v>152</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4792,7 +4847,7 @@
     <x:mergeCell ref="B18:F18"/>
     <x:mergeCell ref="B35:F35"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
220704 hj: css update
</commit_message>
<xml_diff>
--- a/기획/02_WBS, 기능명세서_FDT.xlsx
+++ b/기획/02_WBS, 기능명세서_FDT.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.4575"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11820" activeTab="3"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28605" windowHeight="12030" activeTab="3"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="WBS" sheetId="1" r:id="rId4"/>
@@ -17,165 +17,222 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="175">
+  <x:si>
+    <x:t>Navbar 페이지연결</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>권한(로그인/팀장 등)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프론트/백엔드 카운팅 필요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통합 기능 테스트 및 디버깅</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인페이지에 유저 추가 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 변경 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크 모아보기(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 생성(팀이 없을 경우)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/teams/create/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/user/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 프로필 수정 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/login/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쪽지 보내기/채팅/오픈챗팅</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 페이지 생성/수정/조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>드롭다운으로 데이터 출력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 수정 페이지(모달)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q. 로그아웃-&gt;마이페이지 가능?.?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/teams/&lt;int: team_pk&gt;/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/password/rest</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지 이동(팀 생성 성공 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지 이동(팀이 있을 경우)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인 페이지 이동(회원 가입 성공 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>원인별 로그인 에러 출력(로그인 실패 시)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 로그아웃 완료 alert창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내용</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>api</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>백엔드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>배포</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>디자인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nav</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀장</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모델링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>X</x:t>
+  </x:si>
+  <x:si>
+    <x:t>조건</x:t>
+  </x:si>
+  <x:si>
+    <x:t>체크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/&lt;int: user_pk&gt;/bookmark/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀원이 모두 모집되었을 경우, 해당 팀 카드는 메인에서 제외</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 수정/조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 팀 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정 페이지</x:t>
+  </x:si>
   <x:si>
     <x:t>개별 사용자 조회</x:t>
   </x:si>
   <x:si>
-    <x:t>마이페이지 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지 수정/조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지 조회</x:t>
-  </x:si>
-  <x:si>
     <x:t>팀장 등록 해제</x:t>
   </x:si>
   <x:si>
-    <x:t>팀원이 모두 모집되었을 경우, 해당 팀 카드는 메인에서 제외</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/accounts/&lt;int: user_pk&gt;/bookmark/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>원인별 로그인 에러 출력(로그인 실패 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지 이동(팀 생성 성공 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 로그아웃 완료 alert창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인 페이지 이동(회원 가입 성공 시)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/teams/&lt;int: team_pk&gt;/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 팀 페이지 이동(팀이 있을 경우)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/password/rest</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q. 로그아웃-&gt;마이페이지 가능?.?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>배포</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>백엔드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내용</x:t>
-  </x:si>
-  <x:si>
-    <x:t>api</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디자인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>O</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nav</x:t>
-  </x:si>
-  <x:si>
-    <x:t>조건</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀장</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>체크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모델링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X</x:t>
+    <x:t>북마크/nav =&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>프로세스/태스크</x:t>
@@ -187,183 +244,129 @@
     <x:t>로그인/회원가입</x:t>
   </x:si>
   <x:si>
+    <x:t>팀 생성 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 멤버 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 페이지 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>나의 프로필 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가 기능 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 페이지 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크 등록 해제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 팀/사용자 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>페이지 전환 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>역도 가능해야함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 변경 페이지</x:t>
+  </x:si>
+  <x:si>
     <x:t>북마크 모아보기</x:t>
   </x:si>
   <x:si>
-    <x:t>역도 가능해야함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 팀/사용자 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 변경 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 등록 해제</x:t>
-  </x:si>
-  <x:si>
     <x:t>개인카드 상세조회</x:t>
   </x:si>
   <x:si>
-    <x:t>팀 페이지 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 멤버 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 페이지 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>페이지 전환 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>나의 프로필 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가 기능 구현</x:t>
+    <x:t>팀이 없는 유저</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개별 멤버 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체/개별 팀 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그아웃 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>개인 카드 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 프로필 수정</x:t>
   </x:si>
   <x:si>
     <x:t>개별 팀 페이지</x:t>
   </x:si>
   <x:si>
+    <x:t>팀 카드 상세조회</x:t>
+  </x:si>
+  <x:si>
     <x:t>원인별 에러 출력</x:t>
   </x:si>
   <x:si>
+    <x:t>팀이 있는 유저</x:t>
+  </x:si>
+  <x:si>
     <x:t>마이 페이지 이동</x:t>
   </x:si>
   <x:si>
+    <x:t>북마크 모아보기 기능</x:t>
+  </x:si>
+  <x:si>
     <x:t>/accounts/&lt;int:user_pk&gt;/mypage/</x:t>
   </x:si>
   <x:si>
-    <x:t>팀이 있는 유저</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개인 카드 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체/개별 팀 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그아웃 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 카드 상세조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀이 없는 유저</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개별 멤버 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 프로필 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 모아보기 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입 페이지</x:t>
+    <x:t>RESTful url/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/accounts/signout/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 메인 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인/로그아웃/회원가입/회원탈퇴</x:t>
   </x:si>
   <x:si>
     <x:t>팀을 만드는 유저가 팀장이 됨</x:t>
   </x:si>
   <x:si>
-    <x:t>RESTful url/view</x:t>
+    <x:t>메인페이지에 해당 팀 추가 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 마이 팀 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>/account/logout/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 마이 페이지로 이동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>전체 사용자 조회/개별 사용자 조회</x:t>
+  </x:si>
+  <x:si>
+    <x:t>성공 시, 완료 alert 창</x:t>
   </x:si>
   <x:si>
     <x:t>전체/개별 멤버 페이지(모달)</x:t>
   </x:si>
   <x:si>
-    <x:t>메인페이지에 해당 팀 추가 확인</x:t>
-  </x:si>
-  <x:si>
     <x:t>/account/signup/</x:t>
   </x:si>
   <x:si>
-    <x:t>/account/logout/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 마이 팀 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
     <x:t>메인 페이지 이동(로그인 성공 시)</x:t>
   </x:si>
   <x:si>
-    <x:t>/accounts/signout/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>전체 사용자 조회/개별 사용자 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인/로그아웃/회원가입/회원탈퇴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 마이 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 메인 페이지로 이동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>성공 시, 완료 alert 창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통합 기능 테스트 및 디버깅</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프론트/백엔드 카운팅 필요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성(팀이 없을 경우)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인페이지에 유저 추가 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 모아보기(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navbar 페이지연결</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/teams/create/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 변경 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>권한(로그인/팀장 등)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 프로필 수정 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 수정 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쪽지 보내기/채팅/오픈챗팅</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/login/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 페이지 생성/수정/조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/account/user/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정 페이지(모달)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>드롭다운으로 데이터 출력</x:t>
-  </x:si>
-  <x:si>
     <x:t>로그인이 필요한 서비스입니다 메시지 알림 수정</x:t>
   </x:si>
   <x:si>
@@ -379,163 +382,163 @@
     <x:t>/accounts/&lt;int: user_pk&gt;/</x:t>
   </x:si>
   <x:si>
+    <x:t>팀 탈퇴 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.3</x:t>
+  </x:si>
+  <x:si>
     <x:t>2.2.1</x:t>
   </x:si>
   <x:si>
+    <x:t>1.3.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인여부</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프론트엔드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소셜 로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>check</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호 찾기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그아웃</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>북마크 기능</x:t>
+  </x:si>
+  <x:si>
     <x:t>개별 팀 조회</x:t>
   </x:si>
   <x:si>
-    <x:t>팀 탈퇴 기능</x:t>
+    <x:t>부가기능 3</x:t>
   </x:si>
   <x:si>
     <x:t>기능명세서</x:t>
   </x:si>
   <x:si>
-    <x:t>1.3.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인페이지</x:t>
-  </x:si>
-  <x:si>
     <x:t>메인기능</x:t>
   </x:si>
   <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인여부</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>check</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프론트엔드</x:t>
-  </x:si>
-  <x:si>
     <x:t>메인페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>2.2.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소셜 로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호 찾기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그아웃</x:t>
-  </x:si>
-  <x:si>
-    <x:t>북마크 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.3.1</x:t>
+    <x:t>부가기능 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 생성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>footer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>팀 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유저 본인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 여부</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용자 북마크</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부가기능 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>프로필 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.2.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>도착페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인 페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>출발페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이페이지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구현서비스</x:t>
   </x:si>
   <x:si>
     <x:t>비밀번호 변경</x:t>
   </x:si>
   <x:si>
-    <x:t>2.2.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>도착페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 생성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 여부</x:t>
-  </x:si>
-  <x:si>
-    <x:t>출발페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 페이지</x:t>
-  </x:si>
-  <x:si>
     <x:t>회원탈퇴</x:t>
   </x:si>
   <x:si>
+    <x:t>통합 테스트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2.1.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>덤프데이터</x:t>
+  </x:si>
+  <x:si>
     <x:t>마이팀페이지</x:t>
   </x:si>
   <x:si>
-    <x:t>통합 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>덤프데이터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구현서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>팀 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용자 북마크</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 테스트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.2.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능구현</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이 페이지</x:t>
-  </x:si>
-  <x:si>
     <x:t>부가기능 4</x:t>
   </x:si>
   <x:si>
     <x:t>팀 카드 조회</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인 페이지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>프로필 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>footer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부가기능 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.1.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유저 본인</x:t>
   </x:si>
   <x:si>
     <x:t>해당 팀 멤버</x:t>
@@ -2866,7 +2869,7 @@
       <x:c r="F3" s="89"/>
       <x:c r="G3" s="89"/>
       <x:c r="H3" s="89" t="s">
-        <x:v>51</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="I3" s="89"/>
       <x:c r="J3" s="89"/>
@@ -2914,10 +2917,10 @@
     </x:row>
     <x:row r="5" spans="2:14">
       <x:c r="B5" s="6" t="s">
-        <x:v>47</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D5" s="3"/>
       <x:c r="E5" s="3"/>
@@ -2933,10 +2936,10 @@
     </x:row>
     <x:row r="6" spans="2:14">
       <x:c r="B6" s="25" t="s">
-        <x:v>31</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C6" s="9" t="s">
-        <x:v>22</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D6" s="36"/>
       <x:c r="E6" s="16"/>
@@ -2952,10 +2955,10 @@
     </x:row>
     <x:row r="7" spans="2:14">
       <x:c r="B7" s="12" t="s">
-        <x:v>39</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D7" s="9"/>
       <x:c r="E7" s="16"/>
@@ -2971,10 +2974,10 @@
     </x:row>
     <x:row r="8" spans="2:14">
       <x:c r="B8" s="12" t="s">
-        <x:v>25</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>84</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D8" s="9"/>
       <x:c r="E8" s="16"/>
@@ -2990,10 +2993,10 @@
     </x:row>
     <x:row r="9" spans="2:14">
       <x:c r="B9" s="12" t="s">
-        <x:v>140</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>93</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="D9" s="9"/>
       <x:c r="E9" s="16"/>
@@ -3009,10 +3012,10 @@
     </x:row>
     <x:row r="10" spans="2:14">
       <x:c r="B10" s="12" t="s">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>2</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D10" s="9"/>
       <x:c r="E10" s="16"/>
@@ -3029,7 +3032,7 @@
     <x:row r="11" spans="2:14">
       <x:c r="B11" s="12"/>
       <x:c r="C11" s="3" t="s">
-        <x:v>111</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D11" s="9"/>
       <x:c r="E11" s="16"/>
@@ -3046,7 +3049,7 @@
     <x:row r="12" spans="2:14">
       <x:c r="B12" s="12"/>
       <x:c r="C12" s="3" t="s">
-        <x:v>92</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D12" s="9"/>
       <x:c r="E12" s="16"/>
@@ -3063,7 +3066,7 @@
     <x:row r="13" spans="2:14">
       <x:c r="B13" s="12"/>
       <x:c r="C13" s="3" t="s">
-        <x:v>60</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D13" s="9"/>
       <x:c r="E13" s="16"/>
@@ -3080,7 +3083,7 @@
     <x:row r="14" spans="2:14">
       <x:c r="B14" s="12"/>
       <x:c r="C14" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D14" s="9"/>
       <x:c r="E14" s="16"/>
@@ -3114,7 +3117,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="C16" s="10" t="s">
-        <x:v>133</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D16" s="16"/>
       <x:c r="E16" s="37"/>
@@ -3130,10 +3133,10 @@
     </x:row>
     <x:row r="17" spans="2:14">
       <x:c r="B17" s="12" t="s">
-        <x:v>21</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C17" s="3" t="s">
-        <x:v>162</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="D17" s="16"/>
       <x:c r="E17" s="10"/>
@@ -3149,10 +3152,10 @@
     </x:row>
     <x:row r="18" spans="2:14">
       <x:c r="B18" s="12" t="s">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="C18" s="3" t="s">
-        <x:v>93</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="D18" s="16"/>
       <x:c r="E18" s="10"/>
@@ -3168,10 +3171,10 @@
     </x:row>
     <x:row r="19" spans="2:14">
       <x:c r="B19" s="12" t="s">
-        <x:v>155</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C19" s="3" t="s">
-        <x:v>2</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D19" s="16"/>
       <x:c r="E19" s="10"/>
@@ -3187,10 +3190,10 @@
     </x:row>
     <x:row r="20" spans="2:14">
       <x:c r="B20" s="12" t="s">
-        <x:v>157</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C20" s="3" t="s">
-        <x:v>111</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D20" s="16"/>
       <x:c r="E20" s="10"/>
@@ -3206,10 +3209,10 @@
     </x:row>
     <x:row r="21" spans="2:14">
       <x:c r="B21" s="12" t="s">
-        <x:v>160</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="C21" s="3" t="s">
-        <x:v>92</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D21" s="16"/>
       <x:c r="E21" s="10"/>
@@ -3225,10 +3228,10 @@
     </x:row>
     <x:row r="22" spans="2:14">
       <x:c r="B22" s="12" t="s">
-        <x:v>152</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="C22" s="3" t="s">
-        <x:v>60</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D22" s="16"/>
       <x:c r="E22" s="10"/>
@@ -3244,10 +3247,10 @@
     </x:row>
     <x:row r="23" spans="2:14">
       <x:c r="B23" s="12" t="s">
-        <x:v>171</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C23" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D23" s="16"/>
       <x:c r="E23" s="10"/>
@@ -3263,10 +3266,10 @@
     </x:row>
     <x:row r="24" spans="2:14">
       <x:c r="B24" s="12" t="s">
-        <x:v>38</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C24" s="3" t="s">
-        <x:v>32</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D24" s="16"/>
       <x:c r="E24" s="16"/>
@@ -3282,10 +3285,10 @@
     </x:row>
     <x:row r="25" spans="2:14">
       <x:c r="B25" s="12" t="s">
-        <x:v>120</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C25" s="3" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D25" s="16"/>
       <x:c r="E25" s="16"/>
@@ -3301,10 +3304,10 @@
     </x:row>
     <x:row r="26" spans="2:14">
       <x:c r="B26" s="12" t="s">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="C26" s="3" t="s">
-        <x:v>167</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D26" s="16"/>
       <x:c r="E26" s="16"/>
@@ -3320,10 +3323,10 @@
     </x:row>
     <x:row r="27" spans="2:14">
       <x:c r="B27" s="12" t="s">
-        <x:v>135</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C27" s="3" t="s">
-        <x:v>163</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="D27" s="16"/>
       <x:c r="E27" s="16"/>
@@ -3339,10 +3342,10 @@
     </x:row>
     <x:row r="28" spans="2:14">
       <x:c r="B28" s="12" t="s">
-        <x:v>161</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C28" s="3" t="s">
-        <x:v>156</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D28" s="16"/>
       <x:c r="E28" s="16"/>
@@ -3373,10 +3376,10 @@
     </x:row>
     <x:row r="30" spans="2:14">
       <x:c r="B30" s="29" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C30" s="11" t="s">
-        <x:v>68</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D30" s="16"/>
       <x:c r="E30" s="16"/>
@@ -3392,10 +3395,10 @@
     </x:row>
     <x:row r="31" spans="2:14">
       <x:c r="B31" s="12" t="s">
-        <x:v>26</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C31" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="D31" s="16"/>
       <x:c r="E31" s="16"/>
@@ -3411,10 +3414,10 @@
     </x:row>
     <x:row r="32" spans="2:14">
       <x:c r="B32" s="12" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C32" s="3" t="s">
-        <x:v>109</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D32" s="16"/>
       <x:c r="E32" s="16"/>
@@ -3445,10 +3448,10 @@
     </x:row>
     <x:row r="34" spans="2:14">
       <x:c r="B34" s="27" t="s">
-        <x:v>35</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C34" s="28" t="s">
-        <x:v>150</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D34" s="16"/>
       <x:c r="E34" s="16"/>
@@ -3464,10 +3467,10 @@
     </x:row>
     <x:row r="35" spans="2:14">
       <x:c r="B35" s="12" t="s">
-        <x:v>19</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C35" s="3" t="s">
-        <x:v>97</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D35" s="16"/>
       <x:c r="E35" s="16"/>
@@ -3498,10 +3501,10 @@
     </x:row>
     <x:row r="37" spans="2:14">
       <x:c r="B37" s="30" t="s">
-        <x:v>29</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C37" s="31" t="s">
-        <x:v>18</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D37" s="16"/>
       <x:c r="E37" s="16"/>
@@ -3517,10 +3520,10 @@
     </x:row>
     <x:row r="38" spans="2:14" ht="18">
       <x:c r="B38" s="13" t="s">
-        <x:v>41</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C38" s="8" t="s">
-        <x:v>54</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="D38" s="24"/>
       <x:c r="E38" s="24"/>
@@ -3574,91 +3577,91 @@
     <x:row r="1" ht="9.9499999999999993" customHeight="1"/>
     <x:row r="2" spans="2:2">
       <x:c r="B2" s="1" t="s">
-        <x:v>123</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="3" ht="18"/>
     <x:row r="4" spans="2:6">
       <x:c r="B4" s="45" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C4" s="44" t="s">
-        <x:v>48</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D4" s="44" t="s">
-        <x:v>28</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E4" s="47" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F4" s="17"/>
     </x:row>
     <x:row r="5" spans="2:6">
       <x:c r="B5" s="18" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D5" s="16" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E5" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F5" s="20"/>
     </x:row>
     <x:row r="6" spans="2:6">
       <x:c r="B6" s="6" t="s">
-        <x:v>55</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E6" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F6" s="43"/>
     </x:row>
     <x:row r="7" spans="2:6">
       <x:c r="B7" s="6"/>
       <x:c r="C7" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
-        <x:v>87</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="E7" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F7" s="43"/>
     </x:row>
     <x:row r="8" spans="2:6">
       <x:c r="B8" s="6"/>
       <x:c r="C8" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="E8" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F8" s="43"/>
     </x:row>
     <x:row r="9" spans="2:6">
       <x:c r="B9" s="6"/>
       <x:c r="C9" s="3" t="s">
-        <x:v>137</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E9" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F9" s="43"/>
     </x:row>
@@ -3671,39 +3674,39 @@
     </x:row>
     <x:row r="11" spans="2:6">
       <x:c r="B11" s="6" t="s">
-        <x:v>153</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s">
-        <x:v>72</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E11" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F11" s="43"/>
     </x:row>
     <x:row r="12" spans="2:6">
       <x:c r="B12" s="6"/>
       <x:c r="C12" s="3" t="s">
-        <x:v>1</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D12" s="3" t="s">
-        <x:v>72</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E12" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F12" s="43"/>
     </x:row>
     <x:row r="13" spans="2:6">
       <x:c r="B13" s="6"/>
       <x:c r="C13" s="3" t="s">
-        <x:v>148</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="D13" s="3" t="s">
-        <x:v>91</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="E13" s="42"/>
       <x:c r="F13" s="43"/>
@@ -3717,55 +3720,55 @@
     </x:row>
     <x:row r="15" spans="2:6">
       <x:c r="B15" s="32" t="s">
-        <x:v>167</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="C15" s="33" t="s">
-        <x:v>58</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="D15" s="33" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E15" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F15" s="35"/>
     </x:row>
     <x:row r="16" spans="2:6">
       <x:c r="B16" s="32"/>
       <x:c r="C16" s="33" t="s">
-        <x:v>67</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D16" s="33" t="s">
-        <x:v>112</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E16" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F16" s="35"/>
     </x:row>
     <x:row r="17" spans="2:6">
       <x:c r="B17" s="32"/>
       <x:c r="C17" s="33" t="s">
-        <x:v>0</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D17" s="33" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E17" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F17" s="35"/>
     </x:row>
     <x:row r="18" spans="2:6">
       <x:c r="B18" s="32"/>
       <x:c r="C18" s="33" t="s">
-        <x:v>158</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="D18" s="33" t="s">
-        <x:v>9</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E18" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F18" s="35"/>
     </x:row>
@@ -3778,16 +3781,16 @@
     </x:row>
     <x:row r="20" spans="2:6">
       <x:c r="B20" s="32" t="s">
-        <x:v>3</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C20" s="33" t="s">
-        <x:v>121</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="D20" s="33" t="s">
-        <x:v>14</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E20" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F20" s="35"/>
     </x:row>
@@ -3797,10 +3800,10 @@
         <x:v>144</x:v>
       </x:c>
       <x:c r="D21" s="46" t="s">
-        <x:v>103</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E21" s="42" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F21" s="35"/>
     </x:row>
@@ -3838,94 +3841,94 @@
     <x:row r="1" ht="9" customHeight="1"/>
     <x:row r="2" spans="2:2" ht="17.800000000000001">
       <x:c r="B2" s="83" t="s">
-        <x:v>154</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="3" ht="9" customHeight="1"/>
     <x:row r="4" spans="2:5" ht="18.550000000000001">
       <x:c r="B4" s="50" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C4" s="51" t="s">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D4" s="51" t="s">
-        <x:v>105</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E4" s="52" t="s">
-        <x:v>42</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="48"/>
       <x:c r="B5" s="100" t="s">
-        <x:v>167</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="C5" s="61" t="s">
-        <x:v>65</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D5" s="54"/>
       <x:c r="E5" s="64" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="48"/>
       <x:c r="B6" s="101"/>
       <x:c r="C6" s="62" t="s">
-        <x:v>138</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="D6" s="55" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E6" s="63" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="48"/>
       <x:c r="B7" s="101"/>
       <x:c r="C7" s="62" t="s">
-        <x:v>71</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D7" s="55" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E7" s="63" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="48"/>
       <x:c r="B8" s="101"/>
       <x:c r="C8" s="62" t="s">
-        <x:v>99</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D8" s="55" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E8" s="63" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="48"/>
       <x:c r="B9" s="101"/>
       <x:c r="C9" s="62" t="s">
-        <x:v>15</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D9" s="55" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E9" s="63" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="48"/>
       <x:c r="B10" s="101"/>
       <x:c r="C10" s="62" t="s">
-        <x:v>75</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="D10" s="55"/>
       <x:c r="E10" s="65"/>
@@ -3934,7 +3937,7 @@
       <x:c r="A11" s="48"/>
       <x:c r="B11" s="101"/>
       <x:c r="C11" s="62" t="s">
-        <x:v>85</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="D11" s="55"/>
       <x:c r="E11" s="65"/>
@@ -3948,30 +3951,30 @@
     </x:row>
     <x:row r="13" spans="2:5">
       <x:c r="B13" s="103" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C13" s="56" t="s">
-        <x:v>106</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D13" s="56"/>
       <x:c r="E13" s="73" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5">
       <x:c r="B14" s="104"/>
       <x:c r="C14" s="56" t="s">
-        <x:v>90</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="D14" s="56"/>
       <x:c r="E14" s="73" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5">
       <x:c r="B15" s="104"/>
       <x:c r="C15" s="56" t="s">
-        <x:v>10</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D15" s="56"/>
       <x:c r="E15" s="66"/>
@@ -3984,20 +3987,20 @@
     </x:row>
     <x:row r="17" spans="2:5">
       <x:c r="B17" s="106" t="s">
-        <x:v>4</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C17" s="57" t="s">
-        <x:v>13</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D17" s="57"/>
       <x:c r="E17" s="74" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5">
       <x:c r="B18" s="107"/>
       <x:c r="C18" s="57" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D18" s="57"/>
       <x:c r="E18" s="67"/>
@@ -4010,35 +4013,35 @@
     </x:row>
     <x:row r="20" spans="2:5">
       <x:c r="B20" s="109" t="s">
-        <x:v>163</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C20" s="60" t="s">
-        <x:v>67</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D20" s="60" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E20" s="75" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="2:5">
       <x:c r="B21" s="110"/>
       <x:c r="C21" s="60" t="s">
-        <x:v>113</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D21" s="60" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E21" s="68"/>
     </x:row>
     <x:row r="22" spans="2:5">
       <x:c r="B22" s="110"/>
       <x:c r="C22" s="60" t="s">
-        <x:v>101</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D22" s="60" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E22" s="68"/>
     </x:row>
@@ -4050,23 +4053,23 @@
     </x:row>
     <x:row r="24" spans="2:5">
       <x:c r="B24" s="112" t="s">
-        <x:v>5</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C24" s="59" t="s">
-        <x:v>168</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D24" s="59" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E24" s="69"/>
     </x:row>
     <x:row r="25" spans="2:5">
       <x:c r="B25" s="113"/>
       <x:c r="C25" s="59" t="s">
-        <x:v>104</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D25" s="59" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E25" s="69"/>
     </x:row>
@@ -4078,13 +4081,13 @@
     </x:row>
     <x:row r="27" spans="2:5">
       <x:c r="B27" s="115" t="s">
-        <x:v>59</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C27" s="53" t="s">
-        <x:v>141</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="D27" s="53" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E27" s="70"/>
     </x:row>
@@ -4096,13 +4099,13 @@
     </x:row>
     <x:row r="29" spans="2:5">
       <x:c r="B29" s="93" t="s">
-        <x:v>3</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C29" s="58" t="s">
-        <x:v>108</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D29" s="58" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E29" s="71"/>
     </x:row>
@@ -4114,28 +4117,28 @@
     </x:row>
     <x:row r="31" spans="2:5">
       <x:c r="B31" s="95" t="s">
-        <x:v>63</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C31" s="49" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="D31" s="49" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E31" s="76" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="2:5">
       <x:c r="B32" s="95"/>
       <x:c r="C32" s="49" t="s">
-        <x:v>11</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D32" s="49" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E32" s="76" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="2:5">
@@ -4146,14 +4149,14 @@
     </x:row>
     <x:row r="34" spans="2:5">
       <x:c r="B34" s="96" t="s">
-        <x:v>69</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C34" s="81" t="s">
-        <x:v>121</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="D34" s="81"/>
       <x:c r="E34" s="82" t="s">
-        <x:v>98</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="2:5">
@@ -4164,10 +4167,10 @@
     </x:row>
     <x:row r="36" spans="2:5">
       <x:c r="B36" s="98" t="s">
-        <x:v>79</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C36" s="77" t="s">
-        <x:v>64</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D36" s="77"/>
       <x:c r="E36" s="78"/>
@@ -4175,7 +4178,7 @@
     <x:row r="37" spans="2:5" ht="16.75">
       <x:c r="B37" s="99"/>
       <x:c r="C37" s="79" t="s">
-        <x:v>45</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D37" s="79"/>
       <x:c r="E37" s="80"/>
@@ -4204,7 +4207,7 @@
   <x:dimension ref="B2:J49"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E14" activeCellId="0" sqref="E14:E14"/>
+      <x:selection activeCell="C13" activeCellId="0" sqref="C13:C14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -4223,10 +4226,10 @@
   <x:sheetData>
     <x:row r="2" spans="2:3">
       <x:c r="B2" s="84" t="s">
-        <x:v>47</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C2" s="84" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:3">
@@ -4234,7 +4237,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C3" s="86" t="s">
-        <x:v>36</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:3">
@@ -4242,7 +4245,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C4" s="86" t="s">
-        <x:v>169</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:3">
@@ -4250,7 +4253,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="86" t="s">
-        <x:v>20</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:3">
@@ -4258,15 +4261,18 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C6" s="86" t="s">
-        <x:v>134</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="2:3">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="2:6">
       <x:c r="B7" s="84">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C7" s="86" t="s">
-        <x:v>125</x:v>
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F7" s="84" t="s">
+        <x:v>71</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:3">
@@ -4274,7 +4280,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C8" s="86" t="s">
-        <x:v>82</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:3">
@@ -4282,7 +4288,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C9" s="84" t="s">
-        <x:v>77</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:3">
@@ -4290,7 +4296,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C10" s="86" t="s">
-        <x:v>61</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:3">
@@ -4298,7 +4304,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C11" s="86" t="s">
-        <x:v>153</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:3">
@@ -4306,7 +4312,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C12" s="86" t="s">
-        <x:v>168</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="2:3">
@@ -4314,7 +4320,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C13" s="84" t="s">
-        <x:v>3</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:6">
@@ -4322,23 +4328,23 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C14" s="84" t="s">
-        <x:v>62</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F14" s="84" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:3">
       <x:c r="B15" s="84">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C15" s="84" t="s">
-        <x:v>56</x:v>
+      <x:c r="C15" s="86" t="s">
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:6" ht="17.800000000000001">
       <x:c r="B18" s="88" t="s">
-        <x:v>66</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C18" s="88"/>
       <x:c r="D18" s="88"/>
@@ -4347,22 +4353,22 @@
     </x:row>
     <x:row r="19" spans="2:7">
       <x:c r="B19" s="84" t="s">
-        <x:v>47</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C19" s="84" t="s">
-        <x:v>128</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="D19" s="84" t="s">
-        <x:v>37</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E19" s="85" t="s">
-        <x:v>146</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F19" s="85" t="s">
-        <x:v>143</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G19" s="84" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:7">
@@ -4370,13 +4376,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C20" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E20" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G20" s="84" t="s">
-        <x:v>57</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="2:6">
@@ -4384,13 +4390,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C21" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E21" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F21" s="86" t="s">
-        <x:v>147</x:v>
+        <x:v>151</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="2:6">
@@ -4398,13 +4404,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C22" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E22" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F22" s="86" t="s">
-        <x:v>82</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="2:6">
@@ -4412,13 +4418,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C23" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E23" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F23" s="86" t="s">
-        <x:v>165</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="2:6">
@@ -4426,13 +4432,13 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C24" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E24" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F24" s="86" t="s">
-        <x:v>74</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="2:6">
@@ -4440,16 +4446,16 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C25" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D25" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E25" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F25" s="86" t="s">
-        <x:v>76</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="2:6">
@@ -4457,16 +4463,16 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C26" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D26" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E26" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F26" s="86" t="s">
-        <x:v>153</x:v>
+        <x:v>163</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="2:6">
@@ -4474,16 +4480,16 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C27" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D27" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E27" s="86" t="s">
-        <x:v>153</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F27" s="86" t="s">
-        <x:v>168</x:v>
+        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:6">
@@ -4491,16 +4497,16 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C28" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D28" s="84" t="s">
-        <x:v>73</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="E28" s="84" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F28" s="84" t="s">
-        <x:v>149</x:v>
+        <x:v>171</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="2:6">
@@ -4508,16 +4514,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C29" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D29" s="84" t="s">
-        <x:v>40</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E29" s="84" t="s">
-        <x:v>149</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F29" s="84" t="s">
-        <x:v>107</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="2:6">
@@ -4525,16 +4531,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C30" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D30" s="84" t="s">
-        <x:v>78</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E30" s="84" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F30" s="84" t="s">
-        <x:v>63</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="2:6">
@@ -4542,13 +4548,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C31" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E31" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F31" s="86" t="s">
-        <x:v>165</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="2:6">
@@ -4556,18 +4562,18 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C32" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E32" s="86" t="s">
-        <x:v>134</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="F32" s="86" t="s">
-        <x:v>74</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="2:6" ht="17.800000000000001">
       <x:c r="B35" s="88" t="s">
-        <x:v>159</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="C35" s="88"/>
       <x:c r="D35" s="88"/>
@@ -4576,31 +4582,31 @@
     </x:row>
     <x:row r="36" spans="2:10">
       <x:c r="B36" s="84" t="s">
-        <x:v>47</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C36" s="84" t="s">
-        <x:v>145</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D36" s="84" t="s">
-        <x:v>37</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E36" s="84" t="s">
-        <x:v>126</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F36" s="84" t="s">
-        <x:v>132</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G36" s="84" t="s">
-        <x:v>166</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="H36" s="84" t="s">
-        <x:v>130</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="I36" s="84" t="s">
-        <x:v>164</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="J36" s="84" t="s">
-        <x:v>170</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="2:7">
@@ -4608,19 +4614,19 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C37" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D37" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E37" s="84" t="s">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F37" s="87" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G37" s="84" t="s">
-        <x:v>95</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="2:7">
@@ -4628,19 +4634,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C38" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D38" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E38" s="84" t="s">
-        <x:v>138</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="F38" s="84" t="s">
-        <x:v>12</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G38" s="84" t="s">
-        <x:v>95</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="2:10">
@@ -4648,25 +4654,25 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="C39" s="84" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E39" s="84" t="s">
-        <x:v>127</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F39" s="84" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G39" s="84" t="s">
-        <x:v>96</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="H39" s="84" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="I39" s="84" t="s">
-        <x:v>100</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="J39" s="84" t="s">
-        <x:v>114</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="2:7">
@@ -4674,19 +4680,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C40" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D40" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E40" s="84" t="s">
-        <x:v>141</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F40" s="84" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G40" s="84" t="s">
-        <x:v>94</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="2:10">
@@ -4694,28 +4700,28 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C41" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D41" s="84" t="s">
-        <x:v>78</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E41" s="84" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="F41" s="84" t="s">
-        <x:v>83</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G41" s="84" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="H41" s="84" t="s">
-        <x:v>96</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="I41" s="84" t="s">
-        <x:v>89</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="J41" s="84" t="s">
-        <x:v>86</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="2:8">
@@ -4723,22 +4729,22 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C42" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D42" s="84" t="s">
-        <x:v>40</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E42" s="84" t="s">
-        <x:v>80</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F42" s="84" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G42" s="84" t="s">
-        <x:v>96</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="H42" s="84" t="s">
-        <x:v>89</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="2:6">
@@ -4746,16 +4752,16 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C43" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D43" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E43" s="84" t="s">
-        <x:v>153</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F43" s="84" t="s">
-        <x:v>81</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="2:7">
@@ -4763,19 +4769,19 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C44" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D44" s="84" t="s">
-        <x:v>172</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E44" s="84" t="s">
-        <x:v>168</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F44" s="84" t="s">
-        <x:v>70</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="G44" s="84" t="s">
-        <x:v>94</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="2:7">
@@ -4783,16 +4789,16 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C45" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E45" s="84" t="s">
-        <x:v>165</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F45" s="84" t="s">
-        <x:v>139</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G45" s="84" t="s">
-        <x:v>8</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="2:6">
@@ -4800,16 +4806,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C46" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D46" s="84" t="s">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="E46" s="84" t="s">
-        <x:v>3</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F46" s="84" t="s">
-        <x:v>122</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="2:6">
@@ -4817,13 +4823,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C47" s="84" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E47" s="84" t="s">
-        <x:v>74</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F47" s="84" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="2:5">
@@ -4831,7 +4837,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E48" s="84" t="s">
-        <x:v>102</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="2:5">
@@ -4839,7 +4845,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="E49" s="84" t="s">
-        <x:v>151</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>